<commit_message>
Back end Loyalyty completo
</commit_message>
<xml_diff>
--- a/Service.Catalog/wwwroot/layout/excel/loyalty/LealtadesFormulario.xlsx
+++ b/Service.Catalog/wwwroot/layout/excel/loyalty/LealtadesFormulario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lapaxsis-00\source\repos\Nueva carpeta\Service.Catalog\wwwroot\layout\excel\loyalty\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973E7407-238F-4A29-A249-10E58406ABB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A05CB00-C64D-4F4D-A218-B959AD1EB5E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{3229E258-B22D-4941-8A9E-0DA32DA258DE}"/>
+    <workbookView xWindow="2595" yWindow="180" windowWidth="14280" windowHeight="10875" xr2:uid="{3229E258-B22D-4941-8A9E-0DA32DA258DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Lealtades" sheetId="1" r:id="rId1"/>
@@ -110,7 +110,7 @@
     <t>{{Lealtades.CantidadDescuento}}</t>
   </si>
   <si>
-    <t>{{Lealtades.Vigencia}}   -   {{Lealtades.FechaFinal}}</t>
+    <t>{{Lealtades.FechaInicial}}   -   {{Lealtades.FechaFinal}}</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Cambios tipo de dato en lealtades
</commit_message>
<xml_diff>
--- a/Service.Catalog/wwwroot/layout/excel/loyalty/LealtadesFormulario.xlsx
+++ b/Service.Catalog/wwwroot/layout/excel/loyalty/LealtadesFormulario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lapaxsis-00\source\repos\Nueva carpeta\Service.Catalog\wwwroot\layout\excel\loyalty\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E6203A-3ADA-4C25-909B-353CDFC1F326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2DF148-CDCA-481B-ABA6-F2998F085524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="14280" windowHeight="10875" xr2:uid="{3229E258-B22D-4941-8A9E-0DA32DA258DE}"/>
+    <workbookView xWindow="1905" yWindow="195" windowWidth="14865" windowHeight="10875" xr2:uid="{3229E258-B22D-4941-8A9E-0DA32DA258DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Lealtades" sheetId="1" r:id="rId1"/>
@@ -113,10 +113,10 @@
     <t>Lista de Precios</t>
   </si>
   <si>
-    <t>{{Lealtades.IdListaPrecios}}</t>
-  </si>
-  <si>
     <t xml:space="preserve">{{Lealtades.Fecha2}}  </t>
+  </si>
+  <si>
+    <t>{{Lealtades.PrecioLista}}</t>
   </si>
 </sst>
 </file>
@@ -572,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8A4281-45E9-4A26-88B5-8DB32AE336F4}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:C11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,7 +619,7 @@
         <v>12</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F5" s="4"/>
     </row>
@@ -646,7 +646,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="5"/>
     </row>

</xml_diff>